<commit_message>
added info from master
</commit_message>
<xml_diff>
--- a/assets/template.xlsx
+++ b/assets/template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\examples\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41C9AC6-280E-426D-9E87-FA6A99F65304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733DFBC8-63CA-4AE5-9A30-70E9B14805A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="35415" windowHeight="18600" xr2:uid="{824CC228-956E-423D-87FA-D94E82F1E04D}"/>
   </bookViews>
@@ -40,10 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>&lt;#I.Name&gt;</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>&lt;#C.Title&gt;</t>
   </si>
@@ -55,6 +52,24 @@
   </si>
   <si>
     <t>&lt;#C.Total_Output&gt;</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Ratio</t>
+  </si>
+  <si>
+    <t>&lt;#C.Ratio&gt;</t>
+  </si>
+  <si>
+    <t>&lt;#I.Name&gt; - &lt;#I.cnt&gt; workouts</t>
   </si>
 </sst>
 </file>
@@ -64,7 +79,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,11 +89,24 @@
     </font>
     <font>
       <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -89,7 +117,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -97,23 +125,22 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,36 +455,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D08557-A432-4EDF-A45B-C70955AFA422}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.28515625" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" customWidth="1"/>
+    <col min="1" max="1" width="44.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="8" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>